<commit_message>
got supporting entity visulization now differentiates between non-numerical and numerical answers.
</commit_message>
<xml_diff>
--- a/outputs/hits_k_excel/hits_k_zeroshot_bn.xlsx
+++ b/outputs/hits_k_excel/hits_k_zeroshot_bn.xlsx
@@ -453,14 +453,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1149</v>
+        <v>1100</v>
       </c>
       <c r="C2" t="n">
         <v>2951</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>38.94%</t>
+          <t>37.28%</t>
         </is>
       </c>
     </row>
@@ -469,14 +469,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2264</v>
+        <v>2174</v>
       </c>
       <c r="C3" t="n">
         <v>5902</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>38.36%</t>
+          <t>36.83%</t>
         </is>
       </c>
     </row>
@@ -485,14 +485,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3390</v>
+        <v>3266</v>
       </c>
       <c r="C4" t="n">
         <v>8853</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>38.29%</t>
+          <t>36.89%</t>
         </is>
       </c>
     </row>
@@ -501,14 +501,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>4548</v>
+        <v>4376</v>
       </c>
       <c r="C5" t="n">
         <v>11804</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>38.53%</t>
+          <t>37.07%</t>
         </is>
       </c>
     </row>
@@ -517,14 +517,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5684</v>
+        <v>5466</v>
       </c>
       <c r="C6" t="n">
         <v>14755</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>38.52%</t>
+          <t>37.05%</t>
         </is>
       </c>
     </row>
@@ -590,14 +590,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="C3" t="n">
         <v>2900</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>31.66%</t>
+          <t>31.72%</t>
         </is>
       </c>
     </row>
@@ -606,14 +606,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1366</v>
+        <v>1369</v>
       </c>
       <c r="C4" t="n">
         <v>4350</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>31.40%</t>
+          <t>31.47%</t>
         </is>
       </c>
     </row>
@@ -622,14 +622,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1835</v>
+        <v>1839</v>
       </c>
       <c r="C5" t="n">
         <v>5800</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>31.64%</t>
+          <t>31.71%</t>
         </is>
       </c>
     </row>
@@ -638,14 +638,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2297</v>
+        <v>2302</v>
       </c>
       <c r="C6" t="n">
         <v>7250</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>31.68%</t>
+          <t>31.75%</t>
         </is>
       </c>
     </row>
@@ -695,14 +695,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="C2" t="n">
         <v>655</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>31.30%</t>
+          <t>23.82%</t>
         </is>
       </c>
     </row>
@@ -711,14 +711,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>415</v>
+        <v>322</v>
       </c>
       <c r="C3" t="n">
         <v>1310</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>31.68%</t>
+          <t>24.58%</t>
         </is>
       </c>
     </row>
@@ -727,14 +727,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>620</v>
+        <v>492</v>
       </c>
       <c r="C4" t="n">
         <v>1965</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>31.55%</t>
+          <t>25.04%</t>
         </is>
       </c>
     </row>
@@ -743,14 +743,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>835</v>
+        <v>658</v>
       </c>
       <c r="C5" t="n">
         <v>2620</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>31.87%</t>
+          <t>25.11%</t>
         </is>
       </c>
     </row>
@@ -759,14 +759,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1034</v>
+        <v>809</v>
       </c>
       <c r="C6" t="n">
         <v>3275</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>31.57%</t>
+          <t>24.70%</t>
         </is>
       </c>
     </row>
@@ -953,14 +953,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C3" t="n">
         <v>530</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>41.32%</t>
+          <t>41.51%</t>
         </is>
       </c>
     </row>
@@ -969,14 +969,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C4" t="n">
         <v>795</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>41.13%</t>
+          <t>41.26%</t>
         </is>
       </c>
     </row>
@@ -985,14 +985,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C5" t="n">
         <v>1060</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>41.32%</t>
+          <t>41.42%</t>
         </is>
       </c>
     </row>
@@ -1001,14 +1001,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C6" t="n">
         <v>1325</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>42.26%</t>
+          <t>42.42%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
complexity type of question included in hits_k stats
</commit_message>
<xml_diff>
--- a/outputs/hits_k_excel/hits_k_zeroshot_bn.xlsx
+++ b/outputs/hits_k_excel/hits_k_zeroshot_bn.xlsx
@@ -9,10 +9,19 @@
   <sheets>
     <sheet name="Total Hits" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Hits_entity" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Hits_numerical" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Hits_boolean" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Hits_date" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Hits_string" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Hits_intersection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Hits_numerical" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Hits_count" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Hits_comparative" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Hits_boolean" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Hits_yesno" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Hits_date" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Hits_generic" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Hits_ordinal" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Hits_multihop" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Hits_string" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Hits_difference" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Hits_superlative" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,14 +462,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1149</v>
+        <v>1100</v>
       </c>
       <c r="C2" t="n">
         <v>2951</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>38.94%</t>
+          <t>37.28%</t>
         </is>
       </c>
     </row>
@@ -469,14 +478,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2264</v>
+        <v>2174</v>
       </c>
       <c r="C3" t="n">
         <v>5902</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>38.36%</t>
+          <t>36.83%</t>
         </is>
       </c>
     </row>
@@ -485,14 +494,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3390</v>
+        <v>3266</v>
       </c>
       <c r="C4" t="n">
         <v>8853</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>38.29%</t>
+          <t>36.89%</t>
         </is>
       </c>
     </row>
@@ -501,14 +510,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>4548</v>
+        <v>4376</v>
       </c>
       <c r="C5" t="n">
         <v>11804</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>38.53%</t>
+          <t>37.07%</t>
         </is>
       </c>
     </row>
@@ -517,14 +526,740 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5684</v>
+        <v>5466</v>
       </c>
       <c r="C6" t="n">
         <v>14755</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>38.52%</t>
+          <t>37.05%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>195</v>
+      </c>
+      <c r="C2" t="n">
+        <v>542</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>35.98%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>391</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1084</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>36.07%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>577</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1626</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>35.49%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>767</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2168</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>35.38%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>958</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2710</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>35.35%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>66</v>
+      </c>
+      <c r="C2" t="n">
+        <v>241</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>27.39%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>130</v>
+      </c>
+      <c r="C3" t="n">
+        <v>482</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>26.97%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>201</v>
+      </c>
+      <c r="C4" t="n">
+        <v>723</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>27.80%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>271</v>
+      </c>
+      <c r="C5" t="n">
+        <v>964</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>28.11%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>346</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1205</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>28.71%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>47</v>
+      </c>
+      <c r="C2" t="n">
+        <v>299</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>15.72%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>91</v>
+      </c>
+      <c r="C3" t="n">
+        <v>598</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>15.22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>138</v>
+      </c>
+      <c r="C4" t="n">
+        <v>897</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>15.38%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>189</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1196</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15.80%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>241</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1495</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>16.12%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>12.50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8.33%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>32</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9.38%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10.00%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>59</v>
+      </c>
+      <c r="C2" t="n">
+        <v>225</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>26.22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>115</v>
+      </c>
+      <c r="C3" t="n">
+        <v>450</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>25.56%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>177</v>
+      </c>
+      <c r="C4" t="n">
+        <v>675</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>26.22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>238</v>
+      </c>
+      <c r="C5" t="n">
+        <v>900</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>26.44%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>299</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1125</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>26.58%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>74</v>
+      </c>
+      <c r="C2" t="n">
+        <v>251</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>29.48%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>145</v>
+      </c>
+      <c r="C3" t="n">
+        <v>502</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>28.88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>209</v>
+      </c>
+      <c r="C4" t="n">
+        <v>753</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>27.76%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>285</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>28.39%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>350</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1255</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>27.89%</t>
         </is>
       </c>
     </row>
@@ -590,14 +1325,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="C3" t="n">
         <v>2900</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>31.66%</t>
+          <t>31.72%</t>
         </is>
       </c>
     </row>
@@ -606,14 +1341,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1366</v>
+        <v>1369</v>
       </c>
       <c r="C4" t="n">
         <v>4350</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>31.40%</t>
+          <t>31.47%</t>
         </is>
       </c>
     </row>
@@ -622,14 +1357,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1835</v>
+        <v>1839</v>
       </c>
       <c r="C5" t="n">
         <v>5800</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>31.64%</t>
+          <t>31.71%</t>
         </is>
       </c>
     </row>
@@ -638,14 +1373,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2297</v>
+        <v>2302</v>
       </c>
       <c r="C6" t="n">
         <v>7250</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>31.68%</t>
+          <t>31.75%</t>
         </is>
       </c>
     </row>
@@ -695,14 +1430,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>205</v>
+        <v>95</v>
       </c>
       <c r="C2" t="n">
-        <v>655</v>
+        <v>247</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>31.30%</t>
+          <t>38.46%</t>
         </is>
       </c>
     </row>
@@ -711,14 +1446,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>415</v>
+        <v>184</v>
       </c>
       <c r="C3" t="n">
-        <v>1310</v>
+        <v>494</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>31.68%</t>
+          <t>37.25%</t>
         </is>
       </c>
     </row>
@@ -727,14 +1462,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>620</v>
+        <v>281</v>
       </c>
       <c r="C4" t="n">
-        <v>1965</v>
+        <v>741</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>31.55%</t>
+          <t>37.92%</t>
         </is>
       </c>
     </row>
@@ -743,14 +1478,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>835</v>
+        <v>386</v>
       </c>
       <c r="C5" t="n">
-        <v>2620</v>
+        <v>988</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>31.87%</t>
+          <t>39.07%</t>
         </is>
       </c>
     </row>
@@ -759,14 +1494,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1034</v>
+        <v>488</v>
       </c>
       <c r="C6" t="n">
-        <v>3275</v>
+        <v>1235</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>31.57%</t>
+          <t>39.51%</t>
         </is>
       </c>
     </row>
@@ -816,14 +1551,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>357</v>
+        <v>156</v>
       </c>
       <c r="C2" t="n">
-        <v>573</v>
+        <v>655</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>62.30%</t>
+          <t>23.82%</t>
         </is>
       </c>
     </row>
@@ -832,14 +1567,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>710</v>
+        <v>322</v>
       </c>
       <c r="C3" t="n">
-        <v>1146</v>
+        <v>1310</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>61.95%</t>
+          <t>24.58%</t>
         </is>
       </c>
     </row>
@@ -848,14 +1583,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1075</v>
+        <v>492</v>
       </c>
       <c r="C4" t="n">
-        <v>1719</v>
+        <v>1965</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>62.54%</t>
+          <t>25.04%</t>
         </is>
       </c>
     </row>
@@ -864,14 +1599,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1437</v>
+        <v>658</v>
       </c>
       <c r="C5" t="n">
-        <v>2292</v>
+        <v>2620</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>62.70%</t>
+          <t>25.11%</t>
         </is>
       </c>
     </row>
@@ -880,14 +1615,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1789</v>
+        <v>809</v>
       </c>
       <c r="C6" t="n">
-        <v>2865</v>
+        <v>3275</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>62.44%</t>
+          <t>24.70%</t>
         </is>
       </c>
     </row>
@@ -937,14 +1672,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C2" t="n">
-        <v>265</v>
+        <v>400</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>42.26%</t>
+          <t>30.25%</t>
         </is>
       </c>
     </row>
@@ -953,14 +1688,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="C3" t="n">
-        <v>530</v>
+        <v>800</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>41.32%</t>
+          <t>30.12%</t>
         </is>
       </c>
     </row>
@@ -969,14 +1704,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>327</v>
+        <v>364</v>
       </c>
       <c r="C4" t="n">
-        <v>795</v>
+        <v>1200</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>41.13%</t>
+          <t>30.33%</t>
         </is>
       </c>
     </row>
@@ -985,14 +1720,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>438</v>
+        <v>483</v>
       </c>
       <c r="C5" t="n">
-        <v>1060</v>
+        <v>1600</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>41.32%</t>
+          <t>30.19%</t>
         </is>
       </c>
     </row>
@@ -1001,14 +1736,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>560</v>
+        <v>598</v>
       </c>
       <c r="C6" t="n">
-        <v>1325</v>
+        <v>2000</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>42.26%</t>
+          <t>29.90%</t>
         </is>
       </c>
     </row>
@@ -1058,14 +1793,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>346</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>53.47%</t>
         </is>
       </c>
     </row>
@@ -1074,14 +1809,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>369</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>692</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12.50%</t>
+          <t>53.32%</t>
         </is>
       </c>
     </row>
@@ -1090,14 +1825,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>552</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>1038</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8.33%</t>
+          <t>53.18%</t>
         </is>
       </c>
     </row>
@@ -1106,14 +1841,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>730</v>
       </c>
       <c r="C5" t="n">
-        <v>32</v>
+        <v>1384</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9.38%</t>
+          <t>52.75%</t>
         </is>
       </c>
     </row>
@@ -1122,14 +1857,377 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
+        <v>906</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1730</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>52.37%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>357</v>
+      </c>
+      <c r="C2" t="n">
+        <v>573</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>62.30%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>710</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1146</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>61.95%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1075</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1719</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>62.54%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
+      <c r="B5" t="n">
+        <v>1437</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2292</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>62.70%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1789</v>
+      </c>
       <c r="C6" t="n">
-        <v>40</v>
+        <v>2865</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10.00%</t>
+          <t>62.44%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>258</v>
+      </c>
+      <c r="C2" t="n">
+        <v>400</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>64.50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>508</v>
+      </c>
+      <c r="C3" t="n">
+        <v>800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>63.50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>767</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>63.92%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1027</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>64.19%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1280</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>64.00%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>112</v>
+      </c>
+      <c r="C2" t="n">
+        <v>265</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>42.26%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>220</v>
+      </c>
+      <c r="C3" t="n">
+        <v>530</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>41.51%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>328</v>
+      </c>
+      <c r="C4" t="n">
+        <v>795</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>41.26%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>439</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1060</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>41.42%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>562</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1325</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>42.42%</t>
         </is>
       </c>
     </row>

</xml_diff>